<commit_message>
working through reviewer comments
</commit_message>
<xml_diff>
--- a/supplementary_info/study_info_SI_TableS2.xlsx
+++ b/supplementary_info/study_info_SI_TableS2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/therm_var_meta_analysis/supplementary_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{099C3096-9B85-5E47-A253-D8060C6A5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6063802F-01DF-A84C-B476-9E0B1DC6383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="980" windowWidth="27640" windowHeight="16100" xr2:uid="{23F44D89-F88E-1F46-934B-AE81CE2F6C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14:P40"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,7 +1879,7 @@
         <v>27</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>282</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
tidying up repo for revisions
</commit_message>
<xml_diff>
--- a/supplementary_info/study_info_SI_TableS2.xlsx
+++ b/supplementary_info/study_info_SI_TableS2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/therm_var_meta_analysis/supplementary_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6063802F-01DF-A84C-B476-9E0B1DC6383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97143EA-F10E-1344-8C95-8D7684A2B917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="980" windowWidth="27640" windowHeight="16100" xr2:uid="{23F44D89-F88E-1F46-934B-AE81CE2F6C0B}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="27640" windowHeight="13840" activeTab="1" xr2:uid="{23F44D89-F88E-1F46-934B-AE81CE2F6C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="369">
   <si>
     <t>label</t>
   </si>
@@ -884,13 +885,271 @@
   </si>
   <si>
     <t>acute</t>
+  </si>
+  <si>
+    <t>new source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cited </t>
+  </si>
+  <si>
+    <t>cavieres2019</t>
+  </si>
+  <si>
+    <t>coop2021</t>
+  </si>
+  <si>
+    <t>li2021</t>
+  </si>
+  <si>
+    <t>scharf2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure about the experimental design on this one </t>
+  </si>
+  <si>
+    <t>clavijo-baquet2021</t>
+  </si>
+  <si>
+    <t>noer2020</t>
+  </si>
+  <si>
+    <t>cavieres2020</t>
+  </si>
+  <si>
+    <t>sorenson2020</t>
+  </si>
+  <si>
+    <t>double check means</t>
+  </si>
+  <si>
+    <t>khelifa2019</t>
+  </si>
+  <si>
+    <t>xing2019</t>
+  </si>
+  <si>
+    <t>cavieres2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">downloaded </t>
+  </si>
+  <si>
+    <t>nyamukondiwa2018</t>
+  </si>
+  <si>
+    <t>salachan2017</t>
+  </si>
+  <si>
+    <t>acclim?</t>
+  </si>
+  <si>
+    <t>boher2016</t>
+  </si>
+  <si>
+    <t>theys2021</t>
+  </si>
+  <si>
+    <t>delnat2021</t>
+  </si>
+  <si>
+    <t>salachan2022</t>
+  </si>
+  <si>
+    <t>lu2021</t>
+  </si>
+  <si>
+    <t>rowe2021</t>
+  </si>
+  <si>
+    <t>xing2015</t>
+  </si>
+  <si>
+    <t>paitz2010</t>
+  </si>
+  <si>
+    <t>micheli-campbell2012</t>
+  </si>
+  <si>
+    <t>li2013</t>
+  </si>
+  <si>
+    <t>xing2014</t>
+  </si>
+  <si>
+    <t>lv2022</t>
+  </si>
+  <si>
+    <t>unclear</t>
+  </si>
+  <si>
+    <t>dhaliwal2021</t>
+  </si>
+  <si>
+    <t>1 c diff between constant + flux</t>
+  </si>
+  <si>
+    <t>chen2019</t>
+  </si>
+  <si>
+    <t>salinas2019</t>
+  </si>
+  <si>
+    <t>vangansbeke2015</t>
+  </si>
+  <si>
+    <t>stahlschmidt2020</t>
+  </si>
+  <si>
+    <t>morash2018</t>
+  </si>
+  <si>
+    <t>burton2019</t>
+  </si>
+  <si>
+    <t>zak2020</t>
+  </si>
+  <si>
+    <t>kingsolver</t>
+  </si>
+  <si>
+    <t>shama2015</t>
+  </si>
+  <si>
+    <t>caiveries2016</t>
+  </si>
+  <si>
+    <t>sorensen2016</t>
+  </si>
+  <si>
+    <t>salo2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unclear -- the figure legends loook fucked up </t>
+  </si>
+  <si>
+    <t>castellanos2019</t>
+  </si>
+  <si>
+    <t>hall2020</t>
+  </si>
+  <si>
+    <t>maneti2021</t>
+  </si>
+  <si>
+    <t>bock2021</t>
+  </si>
+  <si>
+    <t>bayu2017</t>
+  </si>
+  <si>
+    <t>rismayani2021</t>
+  </si>
+  <si>
+    <t>moore2021</t>
+  </si>
+  <si>
+    <t>tougeron2021</t>
+  </si>
+  <si>
+    <t>shakya2015</t>
+  </si>
+  <si>
+    <t>lin2015</t>
+  </si>
+  <si>
+    <t>smith2019</t>
+  </si>
+  <si>
+    <t>perhaps</t>
+  </si>
+  <si>
+    <t>reyna2017</t>
+  </si>
+  <si>
+    <t>rodrigues2021</t>
+  </si>
+  <si>
+    <t>qu2019</t>
+  </si>
+  <si>
+    <t>gerhard2019</t>
+  </si>
+  <si>
+    <t>marshall2021</t>
+  </si>
+  <si>
+    <t>vajedsamiei2021</t>
+  </si>
+  <si>
+    <t>bestion2021</t>
+  </si>
+  <si>
+    <t>kunze2022</t>
+  </si>
+  <si>
+    <t>fabricioneto2019?</t>
+  </si>
+  <si>
+    <t>? -- unclear if this is the one I already extracted?</t>
+  </si>
+  <si>
+    <t>jenkitkonchai2021</t>
+  </si>
+  <si>
+    <t>auad2015</t>
+  </si>
+  <si>
+    <t>prasifka2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">? -- unclear   </t>
+  </si>
+  <si>
+    <t>cheng2018</t>
+  </si>
+  <si>
+    <t>waqas2020</t>
+  </si>
+  <si>
+    <t>ghafanzar2020</t>
+  </si>
+  <si>
+    <t>ahn2022</t>
+  </si>
+  <si>
+    <t>azaza2010</t>
+  </si>
+  <si>
+    <t>unclear about experimental design</t>
+  </si>
+  <si>
+    <t>guo2010</t>
+  </si>
+  <si>
+    <t>brito2019</t>
+  </si>
+  <si>
+    <t>zhang2022</t>
+  </si>
+  <si>
+    <t>not sure if this was controlled</t>
+  </si>
+  <si>
+    <t>frances2017</t>
+  </si>
+  <si>
+    <t>kramarz2016</t>
+  </si>
+  <si>
+    <t>gavira2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -898,13 +1157,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -919,9 +1191,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC546662-73AA-4948-A500-9060D4F1FBD0}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2573,50 +2847,50 @@
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:16" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="3">
         <v>2018</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="I28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O28" s="1" t="s">
+      <c r="N28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="P28" s="3" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3193,4 +3467,933 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA80C80-4992-6347-9B04-9869F417E2C2}">
+  <dimension ref="A1:E73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" t="s">
+        <v>365</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>314</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
+        <v>314</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>320</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>314</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>324</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>314</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
+        <v>314</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>314</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" t="s">
+        <v>314</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>331</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>339</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>348</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>349</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" t="s">
+        <v>314</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>366</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C30" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>368</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
+        <v>314</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" t="s">
+        <v>329</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" t="s">
+        <v>361</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>286</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>287</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>290</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>302</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>303</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>304</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>306</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>308</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>309</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>312</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>313</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>318</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>327</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>332</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>333</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>334</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>335</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>336</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>337</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>338</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>342</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>343</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>344</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>346</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>347</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>352</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>353</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>356</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>357</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>358</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>359</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>362</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>363</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>367</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
+    <sortCondition ref="C2:C73"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>